<commit_message>
Dodano: -Generowanie pliku połączonego -Generowanie do excel
</commit_message>
<xml_diff>
--- a/buy.xlsx
+++ b/buy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weap\Desktop\Programowanie\python\excel_file_merge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363A014A-AD74-4091-B2F3-ED8064AC05CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DA0287-3014-44C3-AAA1-A800EDC90639}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17925" yWindow="4350" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10875" yWindow="3690" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -373,7 +373,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,7 +457,7 @@
         <v>44106</v>
       </c>
       <c r="C7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -474,7 +474,7 @@
         <v>44107</v>
       </c>
       <c r="C8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>

</xml_diff>